<commit_message>
Séparation des requêtes knex en plusieurs fichiers
</commit_message>
<xml_diff>
--- a/Documentation/Formulaires FPS.xlsx
+++ b/Documentation/Formulaires FPS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlevasseur\Desktop\4D1\backend\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF6E6FA-60D8-49BE-9EEE-B0B1F2B8DC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB07B860-4D6D-4116-B2ED-7FBAC2B5DA24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,9 +138,6 @@
     <t>Date de naissance:</t>
   </si>
   <si>
-    <t xml:space="preserve">L'enseignant doit composer un numéro FPS ayant 6 caractères.   </t>
-  </si>
-  <si>
     <t>Le système, lui attribuera comme 7e caractère la lettre H par défaut.</t>
   </si>
   <si>
@@ -205,6 +202,9 @@
   </si>
   <si>
     <t>Par cases à cocher, il choisi les antécédents qu'ils désirent associer à cette personne.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'enseignant doit composer un numéro FPS ayant 6 chiffres.   </t>
   </si>
 </sst>
 </file>
@@ -630,6 +630,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -642,6 +648,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -658,15 +667,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:AP57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE35" sqref="AE35"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1344,34 +1344,34 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:31" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="47"/>
-      <c r="R2" s="47"/>
-      <c r="S2" s="47"/>
-      <c r="T2" s="47"/>
-      <c r="U2" s="47"/>
-      <c r="V2" s="47"/>
-      <c r="W2" s="47"/>
-      <c r="X2" s="47"/>
-      <c r="Y2" s="47"/>
-      <c r="Z2" s="47"/>
-      <c r="AA2" s="48"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="50"/>
     </row>
     <row r="3" spans="2:31" ht="18.899999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="11"/>
@@ -1721,7 +1721,7 @@
       <c r="Z14" s="3"/>
       <c r="AA14" s="12"/>
       <c r="AE14" s="1" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1758,7 +1758,7 @@
       <c r="Z15" s="3"/>
       <c r="AA15" s="12"/>
       <c r="AE15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1807,13 +1807,13 @@
       <c r="N17" s="3"/>
       <c r="O17" s="10"/>
       <c r="P17" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="32"/>
       <c r="T17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
@@ -1823,7 +1823,7 @@
       <c r="Z17" s="3"/>
       <c r="AA17" s="12"/>
       <c r="AE17" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AG17" s="6"/>
       <c r="AH17" s="6"/>
@@ -1842,15 +1842,15 @@
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="56"/>
-      <c r="P18" s="56"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="56"/>
-      <c r="S18" s="56"/>
-      <c r="T18" s="56"/>
-      <c r="U18" s="56"/>
-      <c r="V18" s="56"/>
-      <c r="W18" s="56"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+      <c r="Q18" s="52"/>
+      <c r="R18" s="52"/>
+      <c r="S18" s="52"/>
+      <c r="T18" s="52"/>
+      <c r="U18" s="52"/>
+      <c r="V18" s="52"/>
+      <c r="W18" s="52"/>
       <c r="X18" s="8"/>
       <c r="Y18" s="8"/>
       <c r="Z18" s="8"/>
@@ -1876,13 +1876,13 @@
       <c r="N19" s="3"/>
       <c r="O19" s="32"/>
       <c r="P19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="32"/>
       <c r="T19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
@@ -1938,7 +1938,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="32"/>
       <c r="P21" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
@@ -2373,13 +2373,13 @@
       <c r="N34" s="3"/>
       <c r="O34" s="32"/>
       <c r="P34" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="Q34" s="3"/>
       <c r="R34" s="3"/>
       <c r="S34" s="32"/>
       <c r="T34" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
@@ -2389,7 +2389,7 @@
       <c r="Z34" s="3"/>
       <c r="AA34" s="12"/>
       <c r="AE34" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="2:34" ht="7.05" customHeight="1" x14ac:dyDescent="0.2">
@@ -2406,18 +2406,18 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="56"/>
-      <c r="P35" s="56"/>
-      <c r="Q35" s="56"/>
-      <c r="R35" s="56"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
       <c r="U35" s="31"/>
       <c r="V35" s="3"/>
-      <c r="W35" s="49"/>
-      <c r="X35" s="49"/>
-      <c r="Y35" s="49"/>
-      <c r="Z35" s="49"/>
+      <c r="W35" s="51"/>
+      <c r="X35" s="51"/>
+      <c r="Y35" s="51"/>
+      <c r="Z35" s="51"/>
       <c r="AA35" s="12"/>
       <c r="AG35" s="6"/>
       <c r="AH35" s="6"/>
@@ -2438,13 +2438,13 @@
       <c r="N36" s="3"/>
       <c r="O36" s="32"/>
       <c r="P36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="Q36" s="3"/>
       <c r="R36" s="3"/>
       <c r="S36" s="32"/>
       <c r="T36" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="U36" s="31"/>
       <c r="V36" s="3"/>
@@ -2505,13 +2505,13 @@
       <c r="N38" s="3"/>
       <c r="O38" s="32"/>
       <c r="P38" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Q38" s="3"/>
       <c r="R38" s="3"/>
       <c r="S38" s="34"/>
       <c r="T38" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="U38" s="31"/>
       <c r="V38" s="3"/>
@@ -2569,13 +2569,13 @@
       <c r="N40" s="3"/>
       <c r="O40" s="34"/>
       <c r="P40" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="Q40" s="3"/>
       <c r="R40" s="3"/>
       <c r="S40" s="34"/>
       <c r="T40" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
@@ -2600,18 +2600,18 @@
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
-      <c r="O41" s="56"/>
-      <c r="P41" s="56"/>
-      <c r="Q41" s="56"/>
-      <c r="R41" s="56"/>
-      <c r="S41" s="56"/>
-      <c r="T41" s="56"/>
+      <c r="O41" s="52"/>
+      <c r="P41" s="52"/>
+      <c r="Q41" s="52"/>
+      <c r="R41" s="52"/>
+      <c r="S41" s="52"/>
+      <c r="T41" s="52"/>
       <c r="U41" s="33"/>
       <c r="V41" s="3"/>
-      <c r="W41" s="49"/>
-      <c r="X41" s="49"/>
-      <c r="Y41" s="49"/>
-      <c r="Z41" s="49"/>
+      <c r="W41" s="51"/>
+      <c r="X41" s="51"/>
+      <c r="Y41" s="51"/>
+      <c r="Z41" s="51"/>
       <c r="AA41" s="12"/>
       <c r="AG41" s="6"/>
       <c r="AH41" s="6"/>
@@ -2632,13 +2632,13 @@
       <c r="N42" s="3"/>
       <c r="O42" s="34"/>
       <c r="P42" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Q42" s="3"/>
       <c r="R42" s="3"/>
       <c r="S42" s="34"/>
       <c r="T42" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="U42" s="33"/>
       <c r="V42" s="3"/>
@@ -2696,7 +2696,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="34"/>
       <c r="P44" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q44" s="3"/>
       <c r="R44" s="3"/>
@@ -2726,18 +2726,18 @@
       <c r="L45" s="3"/>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-      <c r="O45" s="49"/>
-      <c r="P45" s="49"/>
-      <c r="Q45" s="49"/>
+      <c r="O45" s="51"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="51"/>
       <c r="R45" s="3"/>
-      <c r="S45" s="49"/>
-      <c r="T45" s="49"/>
-      <c r="U45" s="49"/>
+      <c r="S45" s="51"/>
+      <c r="T45" s="51"/>
+      <c r="U45" s="51"/>
       <c r="V45" s="3"/>
-      <c r="W45" s="49"/>
-      <c r="X45" s="49"/>
-      <c r="Y45" s="49"/>
-      <c r="Z45" s="49"/>
+      <c r="W45" s="51"/>
+      <c r="X45" s="51"/>
+      <c r="Y45" s="51"/>
+      <c r="Z45" s="51"/>
       <c r="AA45" s="12"/>
       <c r="AG45" s="6"/>
       <c r="AH45" s="6"/>
@@ -2756,18 +2756,18 @@
       <c r="L46" s="3"/>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
-      <c r="O46" s="49"/>
-      <c r="P46" s="49"/>
-      <c r="Q46" s="49"/>
+      <c r="O46" s="51"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="51"/>
       <c r="R46" s="3"/>
-      <c r="S46" s="49"/>
-      <c r="T46" s="49"/>
-      <c r="U46" s="49"/>
+      <c r="S46" s="51"/>
+      <c r="T46" s="51"/>
+      <c r="U46" s="51"/>
       <c r="V46" s="3"/>
-      <c r="W46" s="49"/>
-      <c r="X46" s="49"/>
-      <c r="Y46" s="49"/>
-      <c r="Z46" s="49"/>
+      <c r="W46" s="51"/>
+      <c r="X46" s="51"/>
+      <c r="Y46" s="51"/>
+      <c r="Z46" s="51"/>
       <c r="AA46" s="12"/>
     </row>
     <row r="47" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2784,18 +2784,18 @@
       <c r="L47" s="3"/>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="49"/>
+      <c r="O47" s="51"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="51"/>
       <c r="R47" s="3"/>
-      <c r="S47" s="49"/>
-      <c r="T47" s="49"/>
-      <c r="U47" s="49"/>
+      <c r="S47" s="51"/>
+      <c r="T47" s="51"/>
+      <c r="U47" s="51"/>
       <c r="V47" s="3"/>
-      <c r="W47" s="49"/>
-      <c r="X47" s="49"/>
-      <c r="Y47" s="49"/>
-      <c r="Z47" s="49"/>
+      <c r="W47" s="51"/>
+      <c r="X47" s="51"/>
+      <c r="Y47" s="51"/>
+      <c r="Z47" s="51"/>
       <c r="AA47" s="12"/>
     </row>
     <row r="48" spans="2:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2853,45 +2853,45 @@
       <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
       <c r="AA49" s="12"/>
-      <c r="AE49" s="58"/>
-      <c r="AF49" s="58"/>
-      <c r="AG49" s="58"/>
-      <c r="AH49" s="57"/>
-      <c r="AI49" s="58"/>
-      <c r="AJ49" s="58"/>
-      <c r="AK49" s="58"/>
-      <c r="AL49" s="57"/>
-      <c r="AM49" s="58"/>
-      <c r="AN49" s="58"/>
-      <c r="AO49" s="58"/>
-      <c r="AP49" s="58"/>
+      <c r="AE49" s="47"/>
+      <c r="AF49" s="47"/>
+      <c r="AG49" s="47"/>
+      <c r="AH49" s="46"/>
+      <c r="AI49" s="47"/>
+      <c r="AJ49" s="47"/>
+      <c r="AK49" s="47"/>
+      <c r="AL49" s="46"/>
+      <c r="AM49" s="47"/>
+      <c r="AN49" s="47"/>
+      <c r="AO49" s="47"/>
+      <c r="AP49" s="47"/>
     </row>
     <row r="50" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B50" s="11"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
-      <c r="E50" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="F50" s="51"/>
-      <c r="G50" s="52"/>
+      <c r="E50" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" s="54"/>
+      <c r="G50" s="55"/>
       <c r="H50" s="3"/>
       <c r="I50" s="3"/>
       <c r="J50" s="3"/>
-      <c r="K50" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="L50" s="51"/>
-      <c r="M50" s="52"/>
+      <c r="K50" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="L50" s="54"/>
+      <c r="M50" s="55"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
       <c r="Q50" s="3"/>
-      <c r="R50" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="S50" s="51"/>
-      <c r="T50" s="52"/>
+      <c r="R50" s="53" t="s">
+        <v>56</v>
+      </c>
+      <c r="S50" s="54"/>
+      <c r="T50" s="55"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
@@ -2899,39 +2899,39 @@
       <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
       <c r="AA50" s="12"/>
-      <c r="AE50" s="58"/>
-      <c r="AF50" s="58"/>
-      <c r="AG50" s="58"/>
-      <c r="AH50" s="57"/>
-      <c r="AI50" s="58"/>
-      <c r="AJ50" s="58"/>
-      <c r="AK50" s="58"/>
-      <c r="AL50" s="57"/>
-      <c r="AM50" s="58"/>
-      <c r="AN50" s="58"/>
-      <c r="AO50" s="58"/>
-      <c r="AP50" s="58"/>
+      <c r="AE50" s="47"/>
+      <c r="AF50" s="47"/>
+      <c r="AG50" s="47"/>
+      <c r="AH50" s="46"/>
+      <c r="AI50" s="47"/>
+      <c r="AJ50" s="47"/>
+      <c r="AK50" s="47"/>
+      <c r="AL50" s="46"/>
+      <c r="AM50" s="47"/>
+      <c r="AN50" s="47"/>
+      <c r="AO50" s="47"/>
+      <c r="AP50" s="47"/>
     </row>
     <row r="51" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="11"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
-      <c r="E51" s="53"/>
-      <c r="F51" s="54"/>
-      <c r="G51" s="55"/>
+      <c r="E51" s="56"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="58"/>
       <c r="H51" s="3"/>
       <c r="I51" s="3"/>
       <c r="J51" s="3"/>
-      <c r="K51" s="53"/>
-      <c r="L51" s="54"/>
-      <c r="M51" s="55"/>
+      <c r="K51" s="56"/>
+      <c r="L51" s="57"/>
+      <c r="M51" s="58"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
       <c r="Q51" s="3"/>
-      <c r="R51" s="53"/>
-      <c r="S51" s="54"/>
-      <c r="T51" s="55"/>
+      <c r="R51" s="56"/>
+      <c r="S51" s="57"/>
+      <c r="T51" s="58"/>
       <c r="U51" s="3"/>
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
@@ -2939,18 +2939,18 @@
       <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
       <c r="AA51" s="12"/>
-      <c r="AE51" s="58"/>
-      <c r="AF51" s="58"/>
-      <c r="AG51" s="58"/>
-      <c r="AH51" s="57"/>
-      <c r="AI51" s="58"/>
-      <c r="AJ51" s="58"/>
-      <c r="AK51" s="58"/>
-      <c r="AL51" s="57"/>
-      <c r="AM51" s="58"/>
-      <c r="AN51" s="58"/>
-      <c r="AO51" s="58"/>
-      <c r="AP51" s="58"/>
+      <c r="AE51" s="47"/>
+      <c r="AF51" s="47"/>
+      <c r="AG51" s="47"/>
+      <c r="AH51" s="46"/>
+      <c r="AI51" s="47"/>
+      <c r="AJ51" s="47"/>
+      <c r="AK51" s="47"/>
+      <c r="AL51" s="46"/>
+      <c r="AM51" s="47"/>
+      <c r="AN51" s="47"/>
+      <c r="AO51" s="47"/>
+      <c r="AP51" s="47"/>
     </row>
     <row r="52" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="11"/>
@@ -2979,18 +2979,18 @@
       <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
       <c r="AA52" s="12"/>
-      <c r="AE52" s="58"/>
-      <c r="AF52" s="58"/>
-      <c r="AG52" s="58"/>
-      <c r="AH52" s="57"/>
-      <c r="AI52" s="58"/>
-      <c r="AJ52" s="58"/>
-      <c r="AK52" s="58"/>
-      <c r="AL52" s="57"/>
-      <c r="AM52" s="58"/>
-      <c r="AN52" s="58"/>
-      <c r="AO52" s="58"/>
-      <c r="AP52" s="58"/>
+      <c r="AE52" s="47"/>
+      <c r="AF52" s="47"/>
+      <c r="AG52" s="47"/>
+      <c r="AH52" s="46"/>
+      <c r="AI52" s="47"/>
+      <c r="AJ52" s="47"/>
+      <c r="AK52" s="47"/>
+      <c r="AL52" s="46"/>
+      <c r="AM52" s="47"/>
+      <c r="AN52" s="47"/>
+      <c r="AO52" s="47"/>
+      <c r="AP52" s="47"/>
     </row>
     <row r="53" spans="2:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="13"/>
@@ -3044,6 +3044,15 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="E50:G51"/>
+    <mergeCell ref="K50:M51"/>
+    <mergeCell ref="R50:T51"/>
+    <mergeCell ref="O18:Q18"/>
+    <mergeCell ref="O47:Q47"/>
+    <mergeCell ref="O46:Q46"/>
+    <mergeCell ref="O45:Q45"/>
+    <mergeCell ref="O35:Q35"/>
+    <mergeCell ref="R35:T35"/>
     <mergeCell ref="B2:AA2"/>
     <mergeCell ref="W47:Z47"/>
     <mergeCell ref="W46:Z46"/>
@@ -3057,15 +3066,6 @@
     <mergeCell ref="O41:Q41"/>
     <mergeCell ref="R41:T41"/>
     <mergeCell ref="W41:Z41"/>
-    <mergeCell ref="E50:G51"/>
-    <mergeCell ref="K50:M51"/>
-    <mergeCell ref="R50:T51"/>
-    <mergeCell ref="O18:Q18"/>
-    <mergeCell ref="O47:Q47"/>
-    <mergeCell ref="O46:Q46"/>
-    <mergeCell ref="O45:Q45"/>
-    <mergeCell ref="O35:Q35"/>
-    <mergeCell ref="R35:T35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>